<commit_message>
update outcome for AHC
</commit_message>
<xml_diff>
--- a/outcome/appendix/data/Epidemic/HAV.xlsx
+++ b/outcome/appendix/data/Epidemic/HAV.xlsx
@@ -462,16 +462,16 @@
         <v>1206.32381161668</v>
       </c>
       <c r="C3" t="n">
-        <v>-2432.31371330295</v>
+        <v>-2259.4625302055</v>
       </c>
       <c r="D3" t="n">
-        <v>-4358.49206733536</v>
+        <v>-4094.13899511842</v>
       </c>
       <c r="E3" t="n">
-        <v>4844.96133653631</v>
+        <v>4672.11015343886</v>
       </c>
       <c r="F3" t="n">
-        <v>6771.13969056872</v>
+        <v>6506.78661835178</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -494,16 +494,16 @@
         <v>1531.17397836404</v>
       </c>
       <c r="C4" t="n">
-        <v>-161310.488690436</v>
+        <v>-134833.293399491</v>
       </c>
       <c r="D4" t="n">
-        <v>-247513.657766536</v>
+        <v>-207020.281942183</v>
       </c>
       <c r="E4" t="n">
-        <v>164372.836647164</v>
+        <v>137895.641356219</v>
       </c>
       <c r="F4" t="n">
-        <v>250576.005723264</v>
+        <v>210082.629898911</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -526,16 +526,16 @@
         <v>1410.96982079323</v>
       </c>
       <c r="C5" t="n">
-        <v>-4286091.60082836</v>
+        <v>-3264950.66302722</v>
       </c>
       <c r="D5" t="n">
-        <v>-6555758.36150002</v>
+        <v>-4994058.06395547</v>
       </c>
       <c r="E5" t="n">
-        <v>4288913.54046994</v>
+        <v>3267772.6026688</v>
       </c>
       <c r="F5" t="n">
-        <v>6558580.3011416</v>
+        <v>4996880.00359705</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -558,16 +558,16 @@
         <v>1420.35143810293</v>
       </c>
       <c r="C6" t="n">
-        <v>-121232720.359572</v>
+        <v>-70009457.5620078</v>
       </c>
       <c r="D6" t="n">
-        <v>-185410197.782918</v>
+        <v>-107070977.611786</v>
       </c>
       <c r="E6" t="n">
-        <v>121235561.062448</v>
+        <v>70012298.264884</v>
       </c>
       <c r="F6" t="n">
-        <v>185413038.485794</v>
+        <v>107073818.314662</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
@@ -590,16 +590,16 @@
         <v>1419.43451361272</v>
       </c>
       <c r="C7" t="n">
-        <v>-3079254326.29898</v>
+        <v>-1458319268.08154</v>
       </c>
       <c r="D7" t="n">
-        <v>-4709313853.61965</v>
+        <v>-2230307607.75358</v>
       </c>
       <c r="E7" t="n">
-        <v>3079257165.168</v>
+        <v>1458322106.95057</v>
       </c>
       <c r="F7" t="n">
-        <v>4709316692.48868</v>
+        <v>2230310446.62261</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
@@ -622,16 +622,16 @@
         <v>1519.78312714683</v>
       </c>
       <c r="C8" t="n">
-        <v>-75418049118.4625</v>
+        <v>-46147602939.7709</v>
       </c>
       <c r="D8" t="n">
-        <v>-115341953505.151</v>
+        <v>-70576669092.0543</v>
       </c>
       <c r="E8" t="n">
-        <v>75418052158.0287</v>
+        <v>46147605979.3372</v>
       </c>
       <c r="F8" t="n">
-        <v>115341956544.717</v>
+        <v>70576672131.6206</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
@@ -654,16 +654,16 @@
         <v>1581.25789100461</v>
       </c>
       <c r="C9" t="n">
-        <v>-2046159463904.08</v>
+        <v>-894593910242.707</v>
       </c>
       <c r="D9" t="n">
-        <v>-3129330855482.42</v>
+        <v>-1368163320991.46</v>
       </c>
       <c r="E9" t="n">
-        <v>2046159467066.59</v>
+        <v>894593913405.223</v>
       </c>
       <c r="F9" t="n">
-        <v>3129330858644.93</v>
+        <v>1368163324153.98</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
@@ -686,16 +686,16 @@
         <v>1443.93537716351</v>
       </c>
       <c r="C10" t="n">
-        <v>-29851890756866.8</v>
+        <v>-13290184935575.6</v>
       </c>
       <c r="D10" t="n">
-        <v>-45654527159037.2</v>
+        <v>-20325583864832.7</v>
       </c>
       <c r="E10" t="n">
-        <v>29851890759754.6</v>
+        <v>13290184938463.4</v>
       </c>
       <c r="F10" t="n">
-        <v>45654527161925.1</v>
+        <v>20325583867720.6</v>
       </c>
       <c r="G10" t="s">
         <v>10</v>
@@ -718,16 +718,16 @@
         <v>1379.60468848891</v>
       </c>
       <c r="C11" t="n">
-        <v>-478050750075792</v>
+        <v>-191059760745981</v>
       </c>
       <c r="D11" t="n">
-        <v>-731115530676038</v>
+        <v>-292200688622908</v>
       </c>
       <c r="E11" t="n">
-        <v>478050750078552</v>
+        <v>191059760748740</v>
       </c>
       <c r="F11" t="n">
-        <v>731115530678797</v>
+        <v>292200688625667</v>
       </c>
       <c r="G11" t="s">
         <v>10</v>
@@ -750,16 +750,16 @@
         <v>1342.88674124662</v>
       </c>
       <c r="C12" t="n">
-        <v>-6641568609514528</v>
+        <v>-3441885251514470</v>
       </c>
       <c r="D12" t="n">
-        <v>-10157402655873172</v>
+        <v>-5263909243497454</v>
       </c>
       <c r="E12" t="n">
-        <v>6641568609517214</v>
+        <v>3441885251517156</v>
       </c>
       <c r="F12" t="n">
-        <v>10157402655875856</v>
+        <v>5263909243500140</v>
       </c>
       <c r="G12" t="s">
         <v>10</v>
@@ -782,16 +782,16 @@
         <v>1261.01354591642</v>
       </c>
       <c r="C13" t="n">
-        <v>-104004182908297808</v>
+        <v>-48884675193664472</v>
       </c>
       <c r="D13" t="n">
-        <v>-159060671628266656</v>
+        <v>-74762659070067152</v>
       </c>
       <c r="E13" t="n">
-        <v>104004182908300336</v>
+        <v>48884675193667000</v>
       </c>
       <c r="F13" t="n">
-        <v>159060671628269152</v>
+        <v>74762659070069680</v>
       </c>
       <c r="G13" t="s">
         <v>10</v>
@@ -814,16 +814,16 @@
         <v>1239.5023369375</v>
       </c>
       <c r="C14" t="n">
-        <v>-1275265791743633408</v>
+        <v>-641435031656251520</v>
       </c>
       <c r="D14" t="n">
-        <v>-1950350723087226112</v>
+        <v>-980990226432531456</v>
       </c>
       <c r="E14" t="n">
-        <v>1275265791743635968</v>
+        <v>641435031656254080</v>
       </c>
       <c r="F14" t="n">
-        <v>1950350723087228672</v>
+        <v>980990226432534016</v>
       </c>
       <c r="G14" t="s">
         <v>10</v>
@@ -846,16 +846,16 @@
         <v>1185.24675435992</v>
       </c>
       <c r="C15" t="n">
-        <v>-14516919379292311552</v>
+        <v>-11743091219968165888</v>
       </c>
       <c r="D15" t="n">
-        <v>-22201712295356149760</v>
+        <v>-17959508206386817024</v>
       </c>
       <c r="E15" t="n">
-        <v>14516919379292315648</v>
+        <v>11743091219968169984</v>
       </c>
       <c r="F15" t="n">
-        <v>22201712295356149760</v>
+        <v>17959508206386821120</v>
       </c>
       <c r="G15" t="s">
         <v>10</v>
@@ -878,16 +878,16 @@
         <v>1505.05893222603</v>
       </c>
       <c r="C16" t="n">
-        <v>-262679321507382198272</v>
+        <v>-235429646499791863808</v>
       </c>
       <c r="D16" t="n">
-        <v>-401733354692678582272</v>
+        <v>-360058573091048587264</v>
       </c>
       <c r="E16" t="n">
-        <v>262679321507382198272</v>
+        <v>235429646499791863808</v>
       </c>
       <c r="F16" t="n">
-        <v>401733354692678582272</v>
+        <v>360058573091048587264</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
@@ -910,16 +910,16 @@
         <v>1387.47961530892</v>
       </c>
       <c r="C17" t="n">
-        <v>-3815214695560200585216</v>
+        <v>-2998341017555073761280</v>
       </c>
       <c r="D17" t="n">
-        <v>-5834867357372597141504</v>
+        <v>-4585566875164962979840</v>
       </c>
       <c r="E17" t="n">
-        <v>3815214695560200585216</v>
+        <v>2998341017555073761280</v>
       </c>
       <c r="F17" t="n">
-        <v>5834867357372597141504</v>
+        <v>4585566875164962979840</v>
       </c>
       <c r="G17" t="s">
         <v>10</v>
@@ -942,16 +942,16 @@
         <v>1397.27064241342</v>
       </c>
       <c r="C18" t="n">
-        <v>-63561861080733085335552</v>
+        <v>-51818568801568759480320</v>
       </c>
       <c r="D18" t="n">
-        <v>-97209477837619938197504</v>
+        <v>-79249662137727706988544</v>
       </c>
       <c r="E18" t="n">
-        <v>63561861080733085335552</v>
+        <v>51818568801568759480320</v>
       </c>
       <c r="F18" t="n">
-        <v>97209477837619938197504</v>
+        <v>79249662137727706988544</v>
       </c>
       <c r="G18" t="s">
         <v>10</v>
@@ -974,16 +974,16 @@
         <v>1396.92119032969</v>
       </c>
       <c r="C19" t="n">
-        <v>-967308343763124275380224</v>
+        <v>-650532825827139133636608</v>
       </c>
       <c r="D19" t="n">
-        <v>-1479370449612105098199040</v>
+        <v>-994904101919952656662528</v>
       </c>
       <c r="E19" t="n">
-        <v>967308343763124275380224</v>
+        <v>650532825827139133636608</v>
       </c>
       <c r="F19" t="n">
-        <v>1479370449612105098199040</v>
+        <v>994904101919952656662528</v>
       </c>
       <c r="G19" t="s">
         <v>10</v>
@@ -1006,16 +1006,16 @@
         <v>1496.25653967067</v>
       </c>
       <c r="C20" t="n">
-        <v>-22460136320387329768292352</v>
+        <v>-13054253979073793113456640</v>
       </c>
       <c r="D20" t="n">
-        <v>-34349814287115475084115968</v>
+        <v>-19964758603490528094846976</v>
       </c>
       <c r="E20" t="n">
-        <v>22460136320387329768292352</v>
+        <v>13054253979073793113456640</v>
       </c>
       <c r="F20" t="n">
-        <v>34349814287115475084115968</v>
+        <v>19964758603490528094846976</v>
       </c>
       <c r="G20" t="s">
         <v>10</v>
@@ -1038,16 +1038,16 @@
         <v>1557.36783061766</v>
       </c>
       <c r="C21" t="n">
-        <v>-523491565977729056989249536</v>
+        <v>-218729919502209632708853760</v>
       </c>
       <c r="D21" t="n">
-        <v>-800611261467897984398131200</v>
+        <v>-334518544623287937940848640</v>
       </c>
       <c r="E21" t="n">
-        <v>523491565977729056989249536</v>
+        <v>218729919502209632708853760</v>
       </c>
       <c r="F21" t="n">
-        <v>800611261467897984398131200</v>
+        <v>334518544623287937940848640</v>
       </c>
       <c r="G21" t="s">
         <v>10</v>
@@ -1070,16 +1070,16 @@
         <v>1422.64496694594</v>
       </c>
       <c r="C22" t="n">
-        <v>-5193386768290507848020918272</v>
+        <v>-1381123281610597658227900416</v>
       </c>
       <c r="D22" t="n">
-        <v>-7942599655996448123809431552</v>
+        <v>-2112245783115415137325940736</v>
       </c>
       <c r="E22" t="n">
-        <v>5193386768290507848020918272</v>
+        <v>1381123281610597658227900416</v>
       </c>
       <c r="F22" t="n">
-        <v>7942599655996448123809431552</v>
+        <v>2112245783115415137325940736</v>
       </c>
       <c r="G22" t="s">
         <v>10</v>
@@ -1102,16 +1102,16 @@
         <v>1359.7529967553</v>
       </c>
       <c r="C23" t="n">
-        <v>-64194849501801018290211913728</v>
+        <v>-16679901087838333038929903616</v>
       </c>
       <c r="D23" t="n">
-        <v>-98177550087913503091134038016</v>
+        <v>-25509707355365751431781941248</v>
       </c>
       <c r="E23" t="n">
-        <v>64194849501801018290211913728</v>
+        <v>16679901087838333038929903616</v>
       </c>
       <c r="F23" t="n">
-        <v>98177550087913503091134038016</v>
+        <v>25509707355365751431781941248</v>
       </c>
       <c r="G23" t="s">
         <v>10</v>
@@ -1134,16 +1134,16 @@
         <v>1324.02967891418</v>
       </c>
       <c r="C24" t="n">
-        <v>-538174008732995681014234742784</v>
+        <v>-297334236291593132296133148672</v>
       </c>
       <c r="D24" t="n">
-        <v>-823066119921576130481982799872</v>
+        <v>-454733473213460978513314054144</v>
       </c>
       <c r="E24" t="n">
-        <v>538174008732995681014234742784</v>
+        <v>297334236291593132296133148672</v>
       </c>
       <c r="F24" t="n">
-        <v>823066119921576130481982799872</v>
+        <v>454733473213460978513314054144</v>
       </c>
       <c r="G24" t="s">
         <v>10</v>
@@ -1166,16 +1166,16 @@
         <v>1243.73402371234</v>
       </c>
       <c r="C25" t="n">
-        <v>-12566872923349815342412876218368</v>
+        <v>-2209324518522397984720079028224</v>
       </c>
       <c r="D25" t="n">
-        <v>-19219373601709371855042789769216</v>
+        <v>-3378870271696839287856227680256</v>
       </c>
       <c r="E25" t="n">
-        <v>12566872923349815342412876218368</v>
+        <v>2209324518522397984720079028224</v>
       </c>
       <c r="F25" t="n">
-        <v>19219373601709371855042789769216</v>
+        <v>3378870271696839287856227680256</v>
       </c>
       <c r="G25" t="s">
         <v>10</v>
@@ -1198,16 +1198,16 @@
         <v>1222.92853829365</v>
       </c>
       <c r="C26" t="n">
-        <v>-69965479324375462597587334332416</v>
+        <v>-21030209725819252910236370993152</v>
       </c>
       <c r="D26" t="n">
-        <v>-107002966812797565844974586560512</v>
+        <v>-32162930277732322346150863568896</v>
       </c>
       <c r="E26" t="n">
-        <v>69965479324375462597587334332416</v>
+        <v>21030209725819252910236370993152</v>
       </c>
       <c r="F26" t="n">
-        <v>107002966812797565844974586560512</v>
+        <v>32162930277732322346150863568896</v>
       </c>
       <c r="G26" t="s">
         <v>10</v>
@@ -1230,16 +1230,16 @@
         <v>1169.78236179598</v>
       </c>
       <c r="C27" t="n">
-        <v>-1251756552484387789273813519171584</v>
+        <v>-268083769627904742530085747163136</v>
       </c>
       <c r="D27" t="n">
-        <v>-1914396444312281513155173451563008</v>
+        <v>-409998744831730928958796082446336</v>
       </c>
       <c r="E27" t="n">
-        <v>1251756552484387789273813519171584</v>
+        <v>268083769627904742530085747163136</v>
       </c>
       <c r="F27" t="n">
-        <v>1914396444312281513155173451563008</v>
+        <v>409998744831730928958796082446336</v>
       </c>
       <c r="G27" t="s">
         <v>10</v>
@@ -1262,16 +1262,16 @@
         <v>1485.89813894824</v>
       </c>
       <c r="C28" t="n">
-        <v>-21363295090378997606925426392825856</v>
+        <v>-3170603410933411790391316999831552</v>
       </c>
       <c r="D28" t="n">
-        <v>-32672340383315602576102858868916224</v>
+        <v>-4849019471213048742294523553513472</v>
       </c>
       <c r="E28" t="n">
-        <v>21363295090378997606925426392825856</v>
+        <v>3170603410933411790391316999831552</v>
       </c>
       <c r="F28" t="n">
-        <v>32672340383315602576102858868916224</v>
+        <v>4849019471213048742294523553513472</v>
       </c>
       <c r="G28" t="s">
         <v>10</v>
@@ -1294,16 +1294,16 @@
         <v>1370.24469435142</v>
       </c>
       <c r="C29" t="n">
-        <v>-305608725897814866677137232610983936</v>
+        <v>-20430732287138063752721612052365312</v>
       </c>
       <c r="D29" t="n">
-        <v>-467388213026254876542465871156609024</v>
+        <v>-31246108652330029370034443431968768</v>
       </c>
       <c r="E29" t="n">
-        <v>305608725897814866677137232610983936</v>
+        <v>20430732287138063752721612052365312</v>
       </c>
       <c r="F29" t="n">
-        <v>467388213026254876542465871156609024</v>
+        <v>31246108652330029370034443431968768</v>
       </c>
       <c r="G29" t="s">
         <v>10</v>
@@ -1326,16 +1326,16 @@
         <v>1380.33611647628</v>
       </c>
       <c r="C30" t="n">
-        <v>-4463496087876286506979201762640003072</v>
+        <v>-155643878510921639121038621150281728</v>
       </c>
       <c r="D30" t="n">
-        <v>-6826328188874183694507041702847447040</v>
+        <v>-238036770815303893628755914291937280</v>
       </c>
       <c r="E30" t="n">
-        <v>4463496087876286506979201762640003072</v>
+        <v>155643878510921639121038621150281728</v>
       </c>
       <c r="F30" t="n">
-        <v>6826328188874183694507041702847447040</v>
+        <v>238036770815303893628755914291937280</v>
       </c>
       <c r="G30" t="s">
         <v>10</v>
@@ -1358,16 +1358,16 @@
         <v>1380.40303081201</v>
       </c>
       <c r="C31" t="n">
-        <v>-56578606737947237278512545862816628736</v>
+        <v>-1535861714826426751918995233338032128</v>
       </c>
       <c r="D31" t="n">
-        <v>-86529511947268209122440702011339964416</v>
+        <v>-2348897794849567102297049208757157888</v>
       </c>
       <c r="E31" t="n">
-        <v>56578606737947237278512545862816628736</v>
+        <v>1535861714826426751918995233338032128</v>
       </c>
       <c r="F31" t="n">
-        <v>86529511947268209122440702011339964416</v>
+        <v>2348897794849567102297049208757157888</v>
       </c>
       <c r="G31" t="s">
         <v>10</v>
@@ -1390,16 +1390,16 @@
         <v>1478.99495109704</v>
       </c>
       <c r="C32" t="n">
-        <v>-1273966740358346020706921842995269468160</v>
+        <v>-33293931423363310978883602795213094912</v>
       </c>
       <c r="D32" t="n">
-        <v>-1948363995437957677615125647187276464128</v>
+        <v>-50918674088473458063009433890483863552</v>
       </c>
       <c r="E32" t="n">
-        <v>1273966740358346020706921842995269468160</v>
+        <v>33293931423363310978883602795213094912</v>
       </c>
       <c r="F32" t="n">
-        <v>1948363995437957677615125647187276464128</v>
+        <v>50918674088473458063009433890483863552</v>
       </c>
       <c r="G32" t="s">
         <v>10</v>
@@ -1422,16 +1422,16 @@
         <v>1539.8395692386</v>
       </c>
       <c r="C33" t="n">
-        <v>-37202692491992606654805535396866469920768</v>
+        <v>-302316762311899304240460136433470930944</v>
       </c>
       <c r="D33" t="n">
-        <v>-56896608277512608112504765558436076191744</v>
+        <v>-462353589184123348511284704070074368000</v>
       </c>
       <c r="E33" t="n">
-        <v>37202692491992606654805535396866469920768</v>
+        <v>302316762311899304240460136433470930944</v>
       </c>
       <c r="F33" t="n">
-        <v>56896608277512608112504765558436076191744</v>
+        <v>462353589184123348511284704070074368000</v>
       </c>
       <c r="G33" t="s">
         <v>10</v>
@@ -1454,16 +1454,16 @@
         <v>1407.02409090065</v>
       </c>
       <c r="C34" t="n">
-        <v>-371194453984878719797146813165271540301824</v>
+        <v>-1790821844427718476635682158077791961088</v>
       </c>
       <c r="D34" t="n">
-        <v>-567692928346747067852525116257429710962688</v>
+        <v>-2738825664275438325925865580332119490560</v>
       </c>
       <c r="E34" t="n">
-        <v>371194453984878719797146813165271540301824</v>
+        <v>1790821844427718476635682158077791961088</v>
       </c>
       <c r="F34" t="n">
-        <v>567692928346747067852525116257429710962688</v>
+        <v>2738825664275438325925865580332119490560</v>
       </c>
       <c r="G34" t="s">
         <v>10</v>
@@ -1486,16 +1486,16 @@
         <v>1345.18772349491</v>
       </c>
       <c r="C35" t="n">
-        <v>-2304766582789586803805010779236432277929984</v>
+        <v>-20849649449082023265905827929995570315264</v>
       </c>
       <c r="D35" t="n">
-        <v>-3524836312863785160373937309799208726822912</v>
+        <v>-31886787164214163466702676589175784865792</v>
       </c>
       <c r="E35" t="n">
-        <v>2304766582789586803805010779236432277929984</v>
+        <v>20849649449082023265905827929995570315264</v>
       </c>
       <c r="F35" t="n">
-        <v>3524836312863785160373937309799208726822912</v>
+        <v>31886787164214163466702676589175784865792</v>
       </c>
       <c r="G35" t="s">
         <v>10</v>
@@ -1518,16 +1518,16 @@
         <v>1310.19417753639</v>
       </c>
       <c r="C36" t="n">
-        <v>-20618778069032756548449204690723819071995904</v>
+        <v>-315008357744247608588337944663175060258816</v>
       </c>
       <c r="D36" t="n">
-        <v>-31533699858074175954448468387208092157214720</v>
+        <v>-481763709402879486193156259507139900342272</v>
       </c>
       <c r="E36" t="n">
-        <v>20618778069032756548449204690723819071995904</v>
+        <v>315008357744247608588337944663175060258816</v>
       </c>
       <c r="F36" t="n">
-        <v>31533699858074175954448468387208092157214720</v>
+        <v>481763709402879486193156259507139900342272</v>
       </c>
       <c r="G36" t="s">
         <v>10</v>
@@ -1550,16 +1550,16 @@
         <v>1231.05597723644</v>
       </c>
       <c r="C37" t="n">
-        <v>-470389328760005897623155708674612369909874688</v>
+        <v>-2107601886291681823496989932430573072023552</v>
       </c>
       <c r="D37" t="n">
-        <v>-719398397901997483662058842674509227969478656</v>
+        <v>-3223298930718380298460520843454124369379328</v>
       </c>
       <c r="E37" t="n">
-        <v>470389328760005897623155708674612369909874688</v>
+        <v>2107601886291681823496989932430573072023552</v>
       </c>
       <c r="F37" t="n">
-        <v>719398397901997483662058842674509227969478656</v>
+        <v>3223298930718380298460520843454124369379328</v>
       </c>
       <c r="G37" t="s">
         <v>10</v>
@@ -1582,16 +1582,16 @@
         <v>1210.76829102618</v>
       </c>
       <c r="C38" t="n">
-        <v>-1641358727011571633677138587020435548857696256</v>
+        <v>-17243537129785076039180854424103480796905472</v>
       </c>
       <c r="D38" t="n">
-        <v>-2510241551838073066390238024564906001784897536</v>
+        <v>-26371714294692362621808151243898209020411904</v>
       </c>
       <c r="E38" t="n">
-        <v>1641358727011571633677138587020435548857696256</v>
+        <v>17243537129785076039180854424103480796905472</v>
       </c>
       <c r="F38" t="n">
-        <v>2510241551838073066390238024564906001784897536</v>
+        <v>26371714294692362621808151243898209020411904</v>
       </c>
       <c r="G38" t="s">
         <v>10</v>
@@ -1614,16 +1614,16 @@
         <v>1158.43609622364</v>
       </c>
       <c r="C39" t="n">
-        <v>-29001090114298627481014066487426587747000778752</v>
+        <v>-264078644143409226354275633363778667309694976</v>
       </c>
       <c r="D39" t="n">
-        <v>-44353339861335225227324854152608860294287982592</v>
+        <v>-403873433986483036191041574101648301772242944</v>
       </c>
       <c r="E39" t="n">
-        <v>29001090114298627481014066487426587747000778752</v>
+        <v>264078644143409226354275633363778667309694976</v>
       </c>
       <c r="F39" t="n">
-        <v>44353339861335225227324854152608860294287982592</v>
+        <v>403873433986483036191041574101648301772242944</v>
       </c>
       <c r="G39" t="s">
         <v>10</v>
@@ -1646,16 +1646,16 @@
         <v>1471.83982336644</v>
       </c>
       <c r="C40" t="n">
-        <v>-450489466292198640184602809645840371990138978304</v>
+        <v>-2946581725070109987449624435341535287506370560</v>
       </c>
       <c r="D40" t="n">
-        <v>-688964184575881302804408945268739982111207849984</v>
+        <v>-4506407868330389197191463685184758268429336576</v>
       </c>
       <c r="E40" t="n">
-        <v>450489466292198640184602809645840371990138978304</v>
+        <v>2946581725070109987449624435341535287506370560</v>
       </c>
       <c r="F40" t="n">
-        <v>688964184575881302804408945268739982111207849984</v>
+        <v>4506407868330389197191463685184758268429336576</v>
       </c>
       <c r="G40" t="s">
         <v>10</v>

</xml_diff>